<commit_message>
Adding is_cosmic check, fixing quest items
</commit_message>
<xml_diff>
--- a/resources/data-imports/Locations Give Items/locations_drop_items.xlsx
+++ b/resources/data-imports/Locations Give Items/locations_drop_items.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Locations" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Locations" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -122,6 +122,66 @@
   </si>
   <si>
     <t xml:space="preserve">The dungeons of a child's mind, a broken and shattered mind, contain the evils unspoken</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Frozen Wreck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Ice Plane</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There is a rusted out metal object on what looks like a frozen smooth road. From another time. A yellow line runs down the middle. The rusted out metal object is crumpled, laying - upside down. What is it?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Broken Forest Road</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decorated in lights, there is a smooth rock that runs through this forest, in places there is this yellow paint that is slowly fading into time. All along the road are decorated trees with lights, candy canes, presents and streamers. The Past haunts its echos here.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bloody Snowman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bloody Snowball</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The children would play in the snow. They would create the snowman, false idols according to The Church. Those who participated met a grim fate.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bandits Twsited Arm Port</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twisted Memories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A port formed by a man whos arm was twisted by dark magics performed on him by the Church of God</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Church of God</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A church controlled by the Twsited Bishop who controls the land through persecution and supression of free will.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Twsited grave site</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A grave site of a man unknown and unamed. The land here is twisted, broken and shattered. Who lies burried here?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Federation Controlled Town</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delusional Memories</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The people here are slaves to the Federation. There's the poor and the rich, there is no in between. You either work for The Federation for nothing but scraps, or you are born into a family of one who works for The Federation. Even soldiers sent to die have a higher standing then the people of this town.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delusional Abandoned Gold Mines</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These old Gold Mines hold the memories of the past as haunting apperations.</t>
   </si>
 </sst>
 </file>
@@ -197,8 +257,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -214,282 +286,666 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="12:14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="24.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="32.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="112.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="9.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="4.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="5.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="24.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="32.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="112.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="21.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="23.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="4.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="5.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" s="0" t="n">
+      <c r="G2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" s="0" t="n">
+      <c r="I2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" s="1" t="n">
         <v>32</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="L2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="M2" s="0" t="s">
+      <c r="L2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="0" t="n">
+      <c r="G3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" s="0" t="n">
+      <c r="I3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="1" t="n">
         <v>176</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="1" t="n">
         <v>464</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="M3" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="0" t="n">
+      <c r="G4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I4" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="0" t="n">
+      <c r="I4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1" t="n">
         <v>128</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="M4" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" s="0" t="n">
+      <c r="G5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1" t="n">
         <v>480</v>
       </c>
-      <c r="K5" s="0" t="n">
+      <c r="K5" s="1" t="n">
         <v>176</v>
       </c>
-      <c r="M5" s="0" t="s">
+      <c r="M5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="0" t="n">
+      <c r="G6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I6" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" s="0" t="n">
+      <c r="I6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1" t="n">
         <v>256</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="K6" s="1" t="n">
         <v>224</v>
       </c>
-      <c r="M6" s="0" t="s">
+      <c r="M6" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="0" t="n">
+      <c r="G7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="0" t="n">
+      <c r="I7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="1" t="n">
         <v>208</v>
       </c>
-      <c r="K7" s="0" t="n">
+      <c r="K7" s="1" t="n">
         <v>400</v>
       </c>
-      <c r="M7" s="0" t="s">
+      <c r="M7" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="0" t="n">
+      <c r="G8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" s="0" t="n">
+      <c r="I8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="1" t="n">
         <v>176</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="K8" s="1" t="n">
         <v>352</v>
       </c>
-      <c r="L8" s="0" t="n">
+      <c r="L8" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="M8" s="0" t="s">
-        <v>16</v>
-      </c>
+      <c r="M8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2" t="n">
+        <v>304</v>
+      </c>
+      <c r="K9" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="I10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2" t="n">
+        <v>64</v>
+      </c>
+      <c r="K10" s="2" t="n">
+        <v>416</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="I11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="K11" s="2" t="n">
+        <v>272</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I12" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="3" t="n">
+        <v>448</v>
+      </c>
+      <c r="K12" s="3" t="n">
+        <v>128</v>
+      </c>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="I13" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="3" t="n">
+        <v>384</v>
+      </c>
+      <c r="K13" s="3" t="n">
+        <v>304</v>
+      </c>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="I14" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="3" t="n">
+        <v>384</v>
+      </c>
+      <c r="K14" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N14" s="3"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="I15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J15" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="K15" s="2" t="n">
+        <v>224</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="I16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" s="2" t="n">
+        <v>448</v>
+      </c>
+      <c r="K16" s="2" t="n">
+        <v>320</v>
+      </c>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N16" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
More quests, more npcs, locations, items.
- Lots of various fixes, changes and small adjustments.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Locations Give Items/locations_drop_items.xlsx
+++ b/resources/data-imports/Locations Give Items/locations_drop_items.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -182,6 +182,12 @@
   </si>
   <si>
     <t xml:space="preserve">These old Gold Mines hold the memories of the past as haunting apperations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abandonded Chapel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An old decrepid chapel in the middle of no where. Half burned, half rotted, what remains is a story of the past.</t>
   </si>
 </sst>
 </file>
@@ -397,10 +403,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="12:14"/>
+      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="17:17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -774,108 +780,108 @@
       <c r="N11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3" t="s">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="3" t="n">
+      <c r="F12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="I12" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J12" s="3" t="n">
+      <c r="I12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2" t="n">
         <v>448</v>
       </c>
-      <c r="K12" s="3" t="n">
+      <c r="K12" s="2" t="n">
         <v>128</v>
       </c>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N12" s="3"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="3" t="n">
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="I13" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J13" s="3" t="n">
+      <c r="I13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2" t="n">
         <v>384</v>
       </c>
-      <c r="K13" s="3" t="n">
+      <c r="K13" s="2" t="n">
         <v>304</v>
       </c>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N13" s="3"/>
+      <c r="L13" s="2"/>
+      <c r="M13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3" t="s">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" s="3" t="n">
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="I14" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J14" s="3" t="n">
+      <c r="I14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2" t="n">
         <v>384</v>
       </c>
-      <c r="K14" s="3" t="n">
+      <c r="K14" s="2" t="n">
         <v>32</v>
       </c>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="N14" s="3"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
@@ -946,6 +952,38 @@
         <v>16</v>
       </c>
       <c r="N16" s="2"/>
+    </row>
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="I17" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" s="3" t="n">
+        <v>208</v>
+      </c>
+      <c r="K17" s="3" t="n">
+        <v>416</v>
+      </c>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N17" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>